<commit_message>
need to test bert for comment
</commit_message>
<xml_diff>
--- a/data/Comment 200 label data.xlsx
+++ b/data/Comment 200 label data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qjh/Documents/doctor/重要！！博士项目管理/研究2-自动驾驶弹幕研究/爬取的数据202212/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProject\spider\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00014E23-8179-1A48-8008-174C722F0CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565631F0-7790-45D5-BB5E-6645F4E395AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38490" yWindow="2610" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表 1 - Comment 200 label data" sheetId="1" r:id="rId1"/>
@@ -1470,10 +1470,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2638,26 +2638,26 @@
   </sheetPr>
   <dimension ref="A1:D202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A177" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D202" sqref="D202"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="102.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.33203125" style="1"/>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="102.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.75" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="10" t="s">
         <v>401</v>
       </c>
     </row>
@@ -2686,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20" customHeight="1">
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>30</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1">
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1">
+    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20" customHeight="1">
+    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="20" customHeight="1">
+    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20" customHeight="1">
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20" customHeight="1">
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>46</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="20" customHeight="1">
+    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20" customHeight="1">
+    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>50</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="20" customHeight="1">
+    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>52</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="22.25" customHeight="1">
+    <row r="28" spans="1:4" ht="22.35" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="20" customHeight="1">
+    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>56</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="48.5" customHeight="1">
+    <row r="30" spans="1:4" ht="48.6" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>58</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20" customHeight="1">
+    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>60</v>
       </c>
@@ -3074,8 +3074,11 @@
       <c r="C31" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="20" customHeight="1">
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>62</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="20" customHeight="1">
+    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>64</v>
       </c>
@@ -3103,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="20" customHeight="1">
+    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>66</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="20" customHeight="1">
+    <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>68</v>
       </c>
@@ -3131,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20" customHeight="1">
+    <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>70</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="20" customHeight="1">
+    <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>72</v>
       </c>
@@ -3159,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="20" customHeight="1">
+    <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>74</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20" customHeight="1">
+    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>76</v>
       </c>
@@ -3187,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="20" customHeight="1">
+    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>78</v>
       </c>
@@ -3201,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20" customHeight="1">
+    <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>80</v>
       </c>
@@ -3215,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="20" customHeight="1">
+    <row r="42" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>82</v>
       </c>
@@ -3229,7 +3232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="20" customHeight="1">
+    <row r="43" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>84</v>
       </c>
@@ -3243,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="20" customHeight="1">
+    <row r="44" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>86</v>
       </c>
@@ -3257,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="20" customHeight="1">
+    <row r="45" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>88</v>
       </c>
@@ -3271,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="20" customHeight="1">
+    <row r="46" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>90</v>
       </c>
@@ -3285,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="20" customHeight="1">
+    <row r="47" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>92</v>
       </c>
@@ -3299,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="20" customHeight="1">
+    <row r="48" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>94</v>
       </c>
@@ -3313,7 +3316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="20" customHeight="1">
+    <row r="49" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="6" t="s">
         <v>96</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="20" customHeight="1">
+    <row r="50" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>98</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="20" customHeight="1">
+    <row r="51" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>100</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="20" customHeight="1">
+    <row r="52" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="20" customHeight="1">
+    <row r="53" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>104</v>
       </c>
@@ -3383,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="20" customHeight="1">
+    <row r="54" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="6" t="s">
         <v>106</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="20" customHeight="1">
+    <row r="55" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>108</v>
       </c>
@@ -3411,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="20" customHeight="1">
+    <row r="56" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="6" t="s">
         <v>110</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="20" customHeight="1">
+    <row r="57" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="6" t="s">
         <v>112</v>
       </c>
@@ -3439,7 +3442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="20" customHeight="1">
+    <row r="58" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>114</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="20" customHeight="1">
+    <row r="59" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>116</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="20" customHeight="1">
+    <row r="60" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>72</v>
       </c>
@@ -3481,7 +3484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="20" customHeight="1">
+    <row r="61" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="6" t="s">
         <v>118</v>
       </c>
@@ -3495,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="20" customHeight="1">
+    <row r="62" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="6" t="s">
         <v>120</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="20" customHeight="1">
+    <row r="63" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>122</v>
       </c>
@@ -3523,7 +3526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="20" customHeight="1">
+    <row r="64" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="6" t="s">
         <v>124</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="20" customHeight="1">
+    <row r="65" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="6" t="s">
         <v>126</v>
       </c>
@@ -3551,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="20" customHeight="1">
+    <row r="66" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="6" t="s">
         <v>128</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="20" customHeight="1">
+    <row r="67" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>130</v>
       </c>
@@ -3579,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="48.25" customHeight="1">
+    <row r="68" spans="1:4" ht="48.2" customHeight="1">
       <c r="A68" s="6" t="s">
         <v>132</v>
       </c>
@@ -3593,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="20" customHeight="1">
+    <row r="69" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="6" t="s">
         <v>134</v>
       </c>
@@ -3607,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="20" customHeight="1">
+    <row r="70" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="6" t="s">
         <v>136</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="20" customHeight="1">
+    <row r="71" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A71" s="6" t="s">
         <v>138</v>
       </c>
@@ -3635,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="20" customHeight="1">
+    <row r="72" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="6" t="s">
         <v>140</v>
       </c>
@@ -3649,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="20" customHeight="1">
+    <row r="73" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="6" t="s">
         <v>142</v>
       </c>
@@ -3663,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="20" customHeight="1">
+    <row r="74" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="6" t="s">
         <v>144</v>
       </c>
@@ -3677,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="20" customHeight="1">
+    <row r="75" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A75" s="6" t="s">
         <v>146</v>
       </c>
@@ -3691,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="20" customHeight="1">
+    <row r="76" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A76" s="6" t="s">
         <v>148</v>
       </c>
@@ -3705,7 +3708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="20" customHeight="1">
+    <row r="77" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="6" t="s">
         <v>150</v>
       </c>
@@ -3719,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="20" customHeight="1">
+    <row r="78" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="6" t="s">
         <v>152</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="20" customHeight="1">
+    <row r="79" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="6" t="s">
         <v>154</v>
       </c>
@@ -3747,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="20" customHeight="1">
+    <row r="80" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="6" t="s">
         <v>156</v>
       </c>
@@ -3761,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="20" customHeight="1">
+    <row r="81" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A81" s="6" t="s">
         <v>158</v>
       </c>
@@ -3775,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="20" customHeight="1">
+    <row r="82" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A82" s="6" t="s">
         <v>160</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="20" customHeight="1">
+    <row r="83" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="6" t="s">
         <v>162</v>
       </c>
@@ -3803,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="20" customHeight="1">
+    <row r="84" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="6" t="s">
         <v>164</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="20" customHeight="1">
+    <row r="85" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A85" s="6" t="s">
         <v>166</v>
       </c>
@@ -3831,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="20" customHeight="1">
+    <row r="86" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A86" s="6" t="s">
         <v>168</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="20" customHeight="1">
+    <row r="87" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="6" t="s">
         <v>170</v>
       </c>
@@ -3859,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="20" customHeight="1">
+    <row r="88" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="6" t="s">
         <v>172</v>
       </c>
@@ -3873,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="20" customHeight="1">
+    <row r="89" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="6" t="s">
         <v>174</v>
       </c>
@@ -3887,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="20" customHeight="1">
+    <row r="90" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="6" t="s">
         <v>176</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="20" customHeight="1">
+    <row r="91" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="6" t="s">
         <v>178</v>
       </c>
@@ -3915,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="20" customHeight="1">
+    <row r="92" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="6" t="s">
         <v>180</v>
       </c>
@@ -3929,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="22.25" customHeight="1">
+    <row r="93" spans="1:4" ht="22.35" customHeight="1">
       <c r="A93" s="6" t="s">
         <v>182</v>
       </c>
@@ -3943,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="20" customHeight="1">
+    <row r="94" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="6" t="s">
         <v>183</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="20" customHeight="1">
+    <row r="95" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="6" t="s">
         <v>185</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="20" customHeight="1">
+    <row r="96" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="6" t="s">
         <v>187</v>
       </c>
@@ -3985,7 +3988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="20" customHeight="1">
+    <row r="97" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A97" s="6" t="s">
         <v>189</v>
       </c>
@@ -3999,7 +4002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="20" customHeight="1">
+    <row r="98" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A98" s="6" t="s">
         <v>191</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="20" customHeight="1">
+    <row r="99" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A99" s="6" t="s">
         <v>193</v>
       </c>
@@ -4027,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="20" customHeight="1">
+    <row r="100" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A100" s="6" t="s">
         <v>195</v>
       </c>
@@ -4041,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="48.25" customHeight="1">
+    <row r="101" spans="1:4" ht="48.2" customHeight="1">
       <c r="A101" s="6" t="s">
         <v>197</v>
       </c>
@@ -4055,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="20" customHeight="1">
+    <row r="102" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A102" s="6" t="s">
         <v>199</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="20" customHeight="1">
+    <row r="103" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="6" t="s">
         <v>201</v>
       </c>
@@ -4083,7 +4086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="20" customHeight="1">
+    <row r="104" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A104" s="6" t="s">
         <v>203</v>
       </c>
@@ -4097,7 +4100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="20" customHeight="1">
+    <row r="105" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A105" s="6" t="s">
         <v>205</v>
       </c>
@@ -4111,7 +4114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="20" customHeight="1">
+    <row r="106" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="6" t="s">
         <v>207</v>
       </c>
@@ -4125,7 +4128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="20" customHeight="1">
+    <row r="107" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A107" s="6" t="s">
         <v>209</v>
       </c>
@@ -4139,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="20" customHeight="1">
+    <row r="108" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A108" s="6" t="s">
         <v>211</v>
       </c>
@@ -4153,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="20" customHeight="1">
+    <row r="109" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A109" s="6" t="s">
         <v>213</v>
       </c>
@@ -4167,7 +4170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="20" customHeight="1">
+    <row r="110" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A110" s="6" t="s">
         <v>215</v>
       </c>
@@ -4181,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="20" customHeight="1">
+    <row r="111" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="6" t="s">
         <v>217</v>
       </c>
@@ -4195,7 +4198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="20" customHeight="1">
+    <row r="112" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A112" s="6" t="s">
         <v>219</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="20" customHeight="1">
+    <row r="113" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A113" s="6" t="s">
         <v>221</v>
       </c>
@@ -4223,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="20" customHeight="1">
+    <row r="114" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A114" s="6" t="s">
         <v>223</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="20" customHeight="1">
+    <row r="115" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="6" t="s">
         <v>225</v>
       </c>
@@ -4251,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="20" customHeight="1">
+    <row r="116" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A116" s="6" t="s">
         <v>227</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="20" customHeight="1">
+    <row r="117" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A117" s="6" t="s">
         <v>229</v>
       </c>
@@ -4279,7 +4282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="20" customHeight="1">
+    <row r="118" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A118" s="6" t="s">
         <v>231</v>
       </c>
@@ -4293,7 +4296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="20" customHeight="1">
+    <row r="119" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A119" s="6" t="s">
         <v>233</v>
       </c>
@@ -4307,7 +4310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="20" customHeight="1">
+    <row r="120" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="6" t="s">
         <v>235</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="20" customHeight="1">
+    <row r="121" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="6" t="s">
         <v>237</v>
       </c>
@@ -4335,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="20" customHeight="1">
+    <row r="122" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="6" t="s">
         <v>239</v>
       </c>
@@ -4349,7 +4352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="20" customHeight="1">
+    <row r="123" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A123" s="6" t="s">
         <v>241</v>
       </c>
@@ -4363,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="20" customHeight="1">
+    <row r="124" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A124" s="6" t="s">
         <v>243</v>
       </c>
@@ -4377,7 +4380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="20" customHeight="1">
+    <row r="125" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="6" t="s">
         <v>245</v>
       </c>
@@ -4391,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="20" customHeight="1">
+    <row r="126" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A126" s="6" t="s">
         <v>247</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="20" customHeight="1">
+    <row r="127" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A127" s="6" t="s">
         <v>249</v>
       </c>
@@ -4419,7 +4422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="20" customHeight="1">
+    <row r="128" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A128" s="6" t="s">
         <v>251</v>
       </c>
@@ -4433,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="20" customHeight="1">
+    <row r="129" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A129" s="6" t="s">
         <v>253</v>
       </c>
@@ -4447,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="20" customHeight="1">
+    <row r="130" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A130" s="6" t="s">
         <v>255</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="20" customHeight="1">
+    <row r="131" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A131" s="6" t="s">
         <v>257</v>
       </c>
@@ -4475,7 +4478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="20" customHeight="1">
+    <row r="132" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A132" s="6" t="s">
         <v>259</v>
       </c>
@@ -4489,7 +4492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="20" customHeight="1">
+    <row r="133" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A133" s="6" t="s">
         <v>261</v>
       </c>
@@ -4503,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="20" customHeight="1">
+    <row r="134" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A134" s="6" t="s">
         <v>263</v>
       </c>
@@ -4517,7 +4520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="20" customHeight="1">
+    <row r="135" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A135" s="6" t="s">
         <v>265</v>
       </c>
@@ -4531,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="20" customHeight="1">
+    <row r="136" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A136" s="6" t="s">
         <v>267</v>
       </c>
@@ -4545,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="20" customHeight="1">
+    <row r="137" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A137" s="6" t="s">
         <v>269</v>
       </c>
@@ -4559,7 +4562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="20" customHeight="1">
+    <row r="138" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A138" s="6" t="s">
         <v>271</v>
       </c>
@@ -4573,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="20" customHeight="1">
+    <row r="139" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="6" t="s">
         <v>273</v>
       </c>
@@ -4587,7 +4590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="20" customHeight="1">
+    <row r="140" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A140" s="6" t="s">
         <v>275</v>
       </c>
@@ -4601,7 +4604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="20" customHeight="1">
+    <row r="141" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="6" t="s">
         <v>277</v>
       </c>
@@ -4615,7 +4618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="20" customHeight="1">
+    <row r="142" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A142" s="6" t="s">
         <v>279</v>
       </c>
@@ -4629,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="20" customHeight="1">
+    <row r="143" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A143" s="6" t="s">
         <v>281</v>
       </c>
@@ -4643,7 +4646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="20" customHeight="1">
+    <row r="144" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A144" s="6" t="s">
         <v>283</v>
       </c>
@@ -4657,7 +4660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="20" customHeight="1">
+    <row r="145" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A145" s="6" t="s">
         <v>285</v>
       </c>
@@ -4671,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="20" customHeight="1">
+    <row r="146" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A146" s="6" t="s">
         <v>287</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="20" customHeight="1">
+    <row r="147" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A147" s="6" t="s">
         <v>289</v>
       </c>
@@ -4699,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="20" customHeight="1">
+    <row r="148" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A148" s="6" t="s">
         <v>291</v>
       </c>
@@ -4713,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="20" customHeight="1">
+    <row r="149" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A149" s="6" t="s">
         <v>293</v>
       </c>
@@ -4727,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="20" customHeight="1">
+    <row r="150" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A150" s="6" t="s">
         <v>295</v>
       </c>
@@ -4741,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="20" customHeight="1">
+    <row r="151" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A151" s="6" t="s">
         <v>297</v>
       </c>
@@ -4755,7 +4758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="20" customHeight="1">
+    <row r="152" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A152" s="6" t="s">
         <v>299</v>
       </c>
@@ -4769,7 +4772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="20" customHeight="1">
+    <row r="153" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A153" s="6" t="s">
         <v>301</v>
       </c>
@@ -4783,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="20" customHeight="1">
+    <row r="154" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A154" s="6" t="s">
         <v>303</v>
       </c>
@@ -4797,7 +4800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="20" customHeight="1">
+    <row r="155" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A155" s="6" t="s">
         <v>305</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="20" customHeight="1">
+    <row r="156" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="6" t="s">
         <v>307</v>
       </c>
@@ -4825,7 +4828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="20" customHeight="1">
+    <row r="157" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A157" s="6" t="s">
         <v>309</v>
       </c>
@@ -4839,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="20" customHeight="1">
+    <row r="158" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A158" s="6" t="s">
         <v>311</v>
       </c>
@@ -4853,7 +4856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="20" customHeight="1">
+    <row r="159" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A159" s="6" t="s">
         <v>313</v>
       </c>
@@ -4867,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="20" customHeight="1">
+    <row r="160" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A160" s="6" t="s">
         <v>315</v>
       </c>
@@ -4881,7 +4884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="20" customHeight="1">
+    <row r="161" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A161" s="6" t="s">
         <v>317</v>
       </c>
@@ -4895,7 +4898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="20" customHeight="1">
+    <row r="162" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A162" s="6" t="s">
         <v>319</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="20" customHeight="1">
+    <row r="163" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A163" s="6" t="s">
         <v>321</v>
       </c>
@@ -4923,7 +4926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="20" customHeight="1">
+    <row r="164" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A164" s="6" t="s">
         <v>323</v>
       </c>
@@ -4937,7 +4940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="20" customHeight="1">
+    <row r="165" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A165" s="6" t="s">
         <v>325</v>
       </c>
@@ -4951,7 +4954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="20" customHeight="1">
+    <row r="166" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A166" s="6" t="s">
         <v>327</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="20" customHeight="1">
+    <row r="167" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A167" s="6" t="s">
         <v>329</v>
       </c>
@@ -4979,7 +4982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="20" customHeight="1">
+    <row r="168" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="6" t="s">
         <v>331</v>
       </c>
@@ -4993,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="20" customHeight="1">
+    <row r="169" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A169" s="6" t="s">
         <v>333</v>
       </c>
@@ -5007,7 +5010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="20" customHeight="1">
+    <row r="170" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A170" s="6" t="s">
         <v>335</v>
       </c>
@@ -5021,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="20" customHeight="1">
+    <row r="171" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="6" t="s">
         <v>337</v>
       </c>
@@ -5035,7 +5038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="20" customHeight="1">
+    <row r="172" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A172" s="6" t="s">
         <v>339</v>
       </c>
@@ -5049,7 +5052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="20" customHeight="1">
+    <row r="173" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A173" s="6" t="s">
         <v>341</v>
       </c>
@@ -5063,7 +5066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="20" customHeight="1">
+    <row r="174" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A174" s="6" t="s">
         <v>343</v>
       </c>
@@ -5077,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="20" customHeight="1">
+    <row r="175" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A175" s="6" t="s">
         <v>345</v>
       </c>
@@ -5091,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="20" customHeight="1">
+    <row r="176" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A176" s="6" t="s">
         <v>347</v>
       </c>
@@ -5105,7 +5108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="20" customHeight="1">
+    <row r="177" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A177" s="6" t="s">
         <v>349</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="20" customHeight="1">
+    <row r="178" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A178" s="6" t="s">
         <v>351</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="20" customHeight="1">
+    <row r="179" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A179" s="6" t="s">
         <v>353</v>
       </c>
@@ -5147,7 +5150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="20" customHeight="1">
+    <row r="180" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A180" s="6" t="s">
         <v>355</v>
       </c>
@@ -5161,7 +5164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="20" customHeight="1">
+    <row r="181" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A181" s="6" t="s">
         <v>357</v>
       </c>
@@ -5175,7 +5178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="20" customHeight="1">
+    <row r="182" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A182" s="6" t="s">
         <v>359</v>
       </c>
@@ -5189,7 +5192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="20" customHeight="1">
+    <row r="183" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A183" s="6" t="s">
         <v>361</v>
       </c>
@@ -5203,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="20" customHeight="1">
+    <row r="184" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A184" s="6" t="s">
         <v>363</v>
       </c>
@@ -5217,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="20" customHeight="1">
+    <row r="185" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A185" s="6" t="s">
         <v>365</v>
       </c>
@@ -5231,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="20" customHeight="1">
+    <row r="186" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A186" s="6" t="s">
         <v>367</v>
       </c>
@@ -5245,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="20" customHeight="1">
+    <row r="187" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A187" s="6" t="s">
         <v>369</v>
       </c>
@@ -5259,7 +5262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="20" customHeight="1">
+    <row r="188" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A188" s="6" t="s">
         <v>371</v>
       </c>
@@ -5273,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="20" customHeight="1">
+    <row r="189" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A189" s="6" t="s">
         <v>373</v>
       </c>
@@ -5287,7 +5290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="20" customHeight="1">
+    <row r="190" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A190" s="6" t="s">
         <v>375</v>
       </c>
@@ -5301,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="20" customHeight="1">
+    <row r="191" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A191" s="6" t="s">
         <v>377</v>
       </c>
@@ -5315,7 +5318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="20" customHeight="1">
+    <row r="192" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A192" s="6" t="s">
         <v>379</v>
       </c>
@@ -5329,7 +5332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="20" customHeight="1">
+    <row r="193" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A193" s="6" t="s">
         <v>381</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="20" customHeight="1">
+    <row r="194" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A194" s="6" t="s">
         <v>383</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="20" customHeight="1">
+    <row r="195" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A195" s="6" t="s">
         <v>385</v>
       </c>
@@ -5371,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="20" customHeight="1">
+    <row r="196" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A196" s="6" t="s">
         <v>387</v>
       </c>
@@ -5385,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="20" customHeight="1">
+    <row r="197" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A197" s="6" t="s">
         <v>389</v>
       </c>
@@ -5399,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="20" customHeight="1">
+    <row r="198" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A198" s="6" t="s">
         <v>391</v>
       </c>
@@ -5413,7 +5416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="20" customHeight="1">
+    <row r="199" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A199" s="6" t="s">
         <v>393</v>
       </c>
@@ -5427,7 +5430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="20" customHeight="1">
+    <row r="200" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A200" s="6" t="s">
         <v>395</v>
       </c>
@@ -5441,7 +5444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="20" customHeight="1">
+    <row r="201" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A201" s="6" t="s">
         <v>397</v>
       </c>
@@ -5455,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="20" customHeight="1">
+    <row r="202" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A202" s="6" t="s">
         <v>399</v>
       </c>

</xml_diff>